<commit_message>
add tables of descriptive statistics of macro nutrients
</commit_message>
<xml_diff>
--- a/data/data_out/v2023/nominal_values.xlsx
+++ b/data/data_out/v2023/nominal_values.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="247" uniqueCount="14">
   <si>
     <t>substrate</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>XL [%DM]</t>
+  </si>
+  <si>
+    <t>Substrate</t>
   </si>
 </sst>
 </file>
@@ -113,7 +116,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>8</v>

</xml_diff>